<commit_message>
added fixed lab 6
</commit_message>
<xml_diff>
--- a/lab6/lab_6.xlsx
+++ b/lab6/lab_6.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313AD231-A32E-4835-8308-9E9A866DF2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2584C1F0-B98F-4831-8FF7-D21FC8FAEB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,6 @@
     <sheet name="Лист1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">Лист1!$D$5:$D$7</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
@@ -29,9 +28,8 @@
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">5</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">Лист1!$D$15</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
@@ -51,7 +49,7 @@
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
@@ -431,18 +429,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -451,6 +437,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -747,50 +745,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="9"/>
       <c r="B6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="9"/>
       <c r="B7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+      <c r="A8" s="9"/>
       <c r="B8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -815,30 +813,30 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="13">
         <v>0</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="13">
         <v>85.812499999999986</v>
       </c>
     </row>
@@ -848,70 +846,70 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="14">
         <v>0</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="14">
         <v>0</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="14">
         <v>0</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="14">
         <v>1.6249999999999998</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="13">
         <v>0</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="13">
         <v>0.43750000000000011</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="10" t="s">
         <v>34</v>
       </c>
     </row>
@@ -921,122 +919,122 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="14">
         <v>8.9999999999999982</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F28" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="18">
+      <c r="G28" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="14">
         <v>0</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G29" s="18">
+      <c r="G29" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="14">
         <v>1.6249999999999998</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G30" s="18">
+      <c r="G30" s="14">
         <v>1.6249999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="18">
+      <c r="D31" s="14">
         <v>0.43750000000000011</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F31" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G31" s="18">
+      <c r="G31" s="14">
         <v>0.43750000000000011</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="13">
         <v>5</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G32" s="17">
+      <c r="G32" s="13">
         <v>0</v>
       </c>
     </row>
@@ -1050,25 +1048,26 @@
   <dimension ref="C3:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="3" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="15"/>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
@@ -1136,10 +1135,10 @@
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="12"/>
+      <c r="D14" s="18"/>
     </row>
     <row r="15" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">

</xml_diff>